<commit_message>
updated weight gen, remove blanks
</commit_message>
<xml_diff>
--- a/src/main/scala/producer/CategoryWeight_CalcTool.xlsx
+++ b/src/main/scala/producer/CategoryWeight_CalcTool.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Repos\capstone-team-2\src\main\scala\producer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCEE378F-4006-457B-BCDC-E40020F555FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6337E6A5-97D5-400B-96FC-F3089EACFADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{19E2E3A8-388F-4CD0-96DE-17B50FB33398}"/>
+    <workbookView xWindow="1485" yWindow="150" windowWidth="21900" windowHeight="14205" xr2:uid="{19E2E3A8-388F-4CD0-96DE-17B50FB33398}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Number of categories</t>
   </si>
@@ -59,6 +59,15 @@
   </si>
   <si>
     <t>(Must be equal to 100)</t>
+  </si>
+  <si>
+    <t>usa</t>
+  </si>
+  <si>
+    <t>australia</t>
+  </si>
+  <si>
+    <t>india</t>
   </si>
 </sst>
 </file>
@@ -142,7 +151,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -241,36 +250,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -369,12 +348,12 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1"/>
@@ -382,22 +361,20 @@
     <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="4" fillId="5" borderId="6" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="5" borderId="7" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="5" borderId="8" xfId="4" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="1" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="1" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="3" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="11" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="5" borderId="1" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="3" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="5" borderId="13" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -719,15 +696,15 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.85546875" customWidth="1"/>
     <col min="2" max="2" width="36.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="10"/>
+    <col min="3" max="3" width="18.5703125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="10" customWidth="1"/>
     <col min="7" max="8" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -735,27 +712,29 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16">
+      <c r="B1" s="14">
         <f>COUNT(B4:B19)</f>
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="22" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
+      <c r="A4" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="B4" s="2">
         <v>1.1499999999999999</v>
       </c>
@@ -764,19 +743,21 @@
         <v>0.22330097087378636</v>
       </c>
       <c r="D4" s="11">
-        <f>C4*100</f>
-        <v>22.330097087378636</v>
-      </c>
-      <c r="G4" s="14" t="s">
+        <f>ROUND((C4*100),0)</f>
+        <v>22</v>
+      </c>
+      <c r="G4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="15">
-        <f>SUM(D:D)</f>
-        <v>99.999999999999986</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="H4" s="13">
+        <f>SUM(D4:D19)</f>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="B5" s="3">
         <v>1</v>
       </c>
@@ -784,16 +765,18 @@
         <f>B5/$B$22</f>
         <v>0.1941747572815534</v>
       </c>
-      <c r="D5" s="12">
-        <f t="shared" ref="D5:D19" si="0">C5*100</f>
-        <v>19.417475728155338</v>
-      </c>
-      <c r="G5" s="14" t="s">
+      <c r="D5" s="11">
+        <f t="shared" ref="D5:D19" si="0">ROUND((C5*100),0)</f>
+        <v>19</v>
+      </c>
+      <c r="G5" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="B6" s="3">
         <v>1</v>
       </c>
@@ -801,12 +784,12 @@
         <f>B6/$B$22</f>
         <v>0.1941747572815534</v>
       </c>
-      <c r="D6" s="12">
-        <f t="shared" si="0"/>
-        <v>19.417475728155338</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D6" s="11">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="3">
         <v>1</v>
@@ -815,12 +798,12 @@
         <f>B7/$B$22</f>
         <v>0.1941747572815534</v>
       </c>
-      <c r="D7" s="12">
-        <f t="shared" si="0"/>
-        <v>19.417475728155338</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D7" s="11">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="3">
         <v>1</v>
@@ -829,43 +812,43 @@
         <f>B8/$B$22</f>
         <v>0.1941747572815534</v>
       </c>
-      <c r="D8" s="12">
-        <f t="shared" si="0"/>
-        <v>19.417475728155338</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="11">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="3"/>
       <c r="C9" s="9">
         <f t="shared" ref="C9:C19" si="1">B9/$B$22</f>
         <v>0</v>
       </c>
-      <c r="D9" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="3"/>
       <c r="C10" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D10" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="3"/>
       <c r="C11" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -877,12 +860,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D12" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
+      <c r="D12" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
@@ -891,85 +874,85 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D13" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="22" t="s">
+      <c r="D13" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="23" t="s">
+      <c r="H13" s="20" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="3"/>
       <c r="C14" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D14" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="20">
+      <c r="D14" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="17" t="str">
         <f t="shared" ref="G14:G29" si="2">A4</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="21">
+        <v>usa</v>
+      </c>
+      <c r="H14" s="18">
         <f t="shared" ref="H14:H29" si="3">D4</f>
-        <v>22.330097087378636</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="3"/>
       <c r="C15" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D15" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="18">
-        <f t="shared" si="3"/>
-        <v>19.417475728155338</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D15" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>australia</v>
+      </c>
+      <c r="H15" s="15">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="3"/>
       <c r="C16" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D16" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="18">
-        <f t="shared" si="3"/>
-        <v>19.417475728155338</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D16" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>india</v>
+      </c>
+      <c r="H16" s="15">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="3"/>
       <c r="C17" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -977,19 +960,19 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H17" s="18">
-        <f t="shared" si="3"/>
-        <v>19.417475728155338</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="15">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="3"/>
       <c r="C18" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -997,9 +980,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H18" s="18">
-        <f t="shared" si="3"/>
-        <v>19.417475728155338</v>
+      <c r="H18" s="15">
+        <f t="shared" si="3"/>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1009,7 +992,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1017,7 +1000,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H19" s="18">
+      <c r="H19" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1027,7 +1010,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H20" s="18">
+      <c r="H20" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1040,7 +1023,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H21" s="18">
+      <c r="H21" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1054,7 +1037,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H22" s="18">
+      <c r="H22" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1064,7 +1047,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H23" s="18">
+      <c r="H23" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1074,7 +1057,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H24" s="18">
+      <c r="H24" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1084,7 +1067,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H25" s="18">
+      <c r="H25" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1094,7 +1077,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H26" s="18">
+      <c r="H26" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1104,7 +1087,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H27" s="18">
+      <c r="H27" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1114,7 +1097,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H28" s="18">
+      <c r="H28" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1124,7 +1107,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H29" s="18">
+      <c r="H29" s="15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
random date time generator, complete
</commit_message>
<xml_diff>
--- a/src/main/scala/producer/CategoryWeight_CalcTool.xlsx
+++ b/src/main/scala/producer/CategoryWeight_CalcTool.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Repos\capstone-team-2\src\main\scala\producer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6337E6A5-97D5-400B-96FC-F3089EACFADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4F1B266-7BA0-405C-9146-AAA481A5544F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1485" yWindow="150" windowWidth="21900" windowHeight="14205" xr2:uid="{19E2E3A8-388F-4CD0-96DE-17B50FB33398}"/>
+    <workbookView xWindow="1950" yWindow="420" windowWidth="21900" windowHeight="14205" xr2:uid="{19E2E3A8-388F-4CD0-96DE-17B50FB33398}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Number of categories</t>
   </si>
@@ -61,13 +62,25 @@
     <t>(Must be equal to 100)</t>
   </si>
   <si>
-    <t>usa</t>
-  </si>
-  <si>
-    <t>australia</t>
-  </si>
-  <si>
-    <t>india</t>
+    <t>mon</t>
+  </si>
+  <si>
+    <t>tues</t>
+  </si>
+  <si>
+    <t>wed</t>
+  </si>
+  <si>
+    <t>thurs</t>
+  </si>
+  <si>
+    <t>fri</t>
+  </si>
+  <si>
+    <t>sat</t>
+  </si>
+  <si>
+    <t>sun</t>
   </si>
 </sst>
 </file>
@@ -693,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB9F26A-2AE7-496D-BE69-6E792DC02340}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B7" sqref="B7:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,7 +727,7 @@
       </c>
       <c r="B1" s="14">
         <f>COUNT(B4:B19)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -736,22 +749,22 @@
         <v>8</v>
       </c>
       <c r="B4" s="2">
-        <v>1.1499999999999999</v>
+        <v>1</v>
       </c>
       <c r="C4" s="9">
         <f>B4/$B$22</f>
-        <v>0.22330097087378636</v>
+        <v>0.12030075187969924</v>
       </c>
       <c r="D4" s="11">
         <f>ROUND((C4*100),0)</f>
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="G4" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H4" s="13">
         <f>SUM(D4:D19)</f>
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -759,15 +772,16 @@
         <v>9</v>
       </c>
       <c r="B5" s="3">
-        <v>1</v>
+        <f>B4*1.25</f>
+        <v>1.25</v>
       </c>
       <c r="C5" s="9">
         <f>B5/$B$22</f>
-        <v>0.1941747572815534</v>
+        <v>0.15037593984962405</v>
       </c>
       <c r="D5" s="11">
         <f t="shared" ref="D5:D19" si="0">ROUND((C5*100),0)</f>
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>7</v>
@@ -778,11 +792,12 @@
         <v>10</v>
       </c>
       <c r="B6" s="3">
-        <v>1</v>
+        <f>B5*1.25</f>
+        <v>1.5625</v>
       </c>
       <c r="C6" s="9">
         <f>B6/$B$22</f>
-        <v>0.1941747572815534</v>
+        <v>0.18796992481203006</v>
       </c>
       <c r="D6" s="11">
         <f t="shared" si="0"/>
@@ -790,55 +805,67 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
+      <c r="A7" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="B7" s="3">
         <v>1</v>
       </c>
       <c r="C7" s="9">
         <f>B7/$B$22</f>
-        <v>0.1941747572815534</v>
+        <v>0.12030075187969924</v>
       </c>
       <c r="D7" s="11">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
+      <c r="A8" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="B8" s="3">
         <v>1</v>
       </c>
       <c r="C8" s="9">
         <f>B8/$B$22</f>
-        <v>0.1941747572815534</v>
+        <v>0.12030075187969924</v>
       </c>
       <c r="D8" s="11">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="3"/>
+      <c r="A9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1.25</v>
+      </c>
       <c r="C9" s="9">
         <f t="shared" ref="C9:C19" si="1">B9/$B$22</f>
-        <v>0</v>
+        <v>0.15037593984962405</v>
       </c>
       <c r="D9" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="3"/>
+      <c r="A10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1.25</v>
+      </c>
       <c r="C10" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.15037593984962405</v>
       </c>
       <c r="D10" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -898,11 +925,11 @@
       </c>
       <c r="G14" s="17" t="str">
         <f t="shared" ref="G14:G29" si="2">A4</f>
-        <v>usa</v>
+        <v>mon</v>
       </c>
       <c r="H14" s="18">
         <f t="shared" ref="H14:H29" si="3">D4</f>
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -918,11 +945,11 @@
       </c>
       <c r="G15" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>australia</v>
+        <v>tues</v>
       </c>
       <c r="H15" s="15">
         <f t="shared" si="3"/>
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -938,14 +965,14 @@
       </c>
       <c r="G16" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>india</v>
+        <v>wed</v>
       </c>
       <c r="H16" s="15">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="3"/>
       <c r="C17" s="9">
@@ -956,16 +983,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G17" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
+      <c r="G17" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>thurs</v>
       </c>
       <c r="H17" s="15">
         <f t="shared" si="3"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="3"/>
       <c r="C18" s="9">
@@ -976,16 +1003,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G18" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
+      <c r="G18" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>fri</v>
       </c>
       <c r="H18" s="15">
         <f t="shared" si="3"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="4"/>
       <c r="C19" s="9">
@@ -996,26 +1023,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G19" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
+      <c r="G19" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>sat</v>
       </c>
       <c r="H19" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G20" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>D9</f>
+        <v>15</v>
+      </c>
+      <c r="I19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G20" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>sun</v>
       </c>
       <c r="H20" s="15">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>5</v>
       </c>
@@ -1028,10 +1058,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
-        <f>SUM(B4:B8)</f>
-        <v>5.15</v>
+        <f>SUM(B4:B19)</f>
+        <v>8.3125</v>
       </c>
       <c r="G22" s="6">
         <f t="shared" si="2"/>
@@ -1042,7 +1072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G23" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1052,7 +1082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G24" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1062,7 +1092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G25" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1072,7 +1102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G26" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1082,7 +1112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G27" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1092,7 +1122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G28" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1102,7 +1132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G29" s="7">
         <f t="shared" si="2"/>
         <v>0</v>

</xml_diff>